<commit_message>
First adaptation to linux + worksite adapt
</commit_message>
<xml_diff>
--- a/Lamia/toolprepro/base2_chantier/sousfiches/Orange.xlsx
+++ b/Lamia/toolprepro/base2_chantier/sousfiches/Orange.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B61302-7F9A-4D68-B823-8FA25D351349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{58B61302-7F9A-4D68-B823-8FA25D351349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9215AF37-1DAE-4B45-BBD2-5F2BCB930A6A}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="498">
   <si>
     <t>1.1.1</t>
   </si>
@@ -1380,6 +1380,156 @@
   </si>
   <si>
     <t>Demande de test réflectométrie</t>
+  </si>
+  <si>
+    <t>4.1 FIBRAGE - Plan de baie SRO</t>
+  </si>
+  <si>
+    <t>TIROIRS DE DISTRIBUTION</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>EMPLACEMENT DU TIROIR VS PLAN DE BAIE SRO &amp; SYNO</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>ETIQUETAGE DES TIROIRS</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>COHERENCE TIROIRS VS SYNO</t>
+  </si>
+  <si>
+    <t>TIROIRS DE TRANSPORT</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>4.1.5</t>
+  </si>
+  <si>
+    <t>4.1.6</t>
+  </si>
+  <si>
+    <t>TIROIR DE STOCKAGE</t>
+  </si>
+  <si>
+    <t>4.1.7</t>
+  </si>
+  <si>
+    <t>4.1.8</t>
+  </si>
+  <si>
+    <t>4.1.9</t>
+  </si>
+  <si>
+    <t>TIROIR FTTE</t>
+  </si>
+  <si>
+    <t>4.1.10</t>
+  </si>
+  <si>
+    <t>PRESENCE &amp; EMPLACEMENT TIROIR</t>
+  </si>
+  <si>
+    <t>COHERENCE TIROIR VS SYNO</t>
+  </si>
+  <si>
+    <t>ETIQUETAGE DU TIROIR</t>
+  </si>
+  <si>
+    <t>COHERENCE TIROIR VS SYNO GENERAL TRANSPORT</t>
+  </si>
+  <si>
+    <t>4.2 FIBRAGE - Plan de baie NRO</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>Référence du NRO</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>COHERENCE FERME 1 VS PLAN DE BAIE NRO &amp; SYNO</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>COHERENCE FERME 3 VS PLAN DE BAIE NRO &amp; SYNO</t>
+  </si>
+  <si>
+    <t>4.2.4</t>
+  </si>
+  <si>
+    <t>COHERENCE FERME 5 VS PLAN DE BAIE NRO &amp; SYNO</t>
+  </si>
+  <si>
+    <t>4.3 FIBRAGE - BPE</t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t>Référence de la BPE</t>
+  </si>
+  <si>
+    <t>4.3.2</t>
+  </si>
+  <si>
+    <t>COHERENCE COORDONNEES GPS VS SYNO</t>
+  </si>
+  <si>
+    <t>4.3.3</t>
+  </si>
+  <si>
+    <t>COHERENCE ADRESSE VS SYNO</t>
+  </si>
+  <si>
+    <t>4.3.4</t>
+  </si>
+  <si>
+    <t>COHERENCE TYPE DE BOITE VS SYNO</t>
+  </si>
+  <si>
+    <t>4.3.5</t>
+  </si>
+  <si>
+    <t>COHERENCE FIBRES EPISSUREES VS PLAN DE SOUDURE</t>
+  </si>
+  <si>
+    <t>4.3.6</t>
+  </si>
+  <si>
+    <t>COHERENCE FIBRES EN ATTENTE RACCO CLIENT  VS PLAN DE SOUDURE</t>
+  </si>
+  <si>
+    <t>4.3.7</t>
+  </si>
+  <si>
+    <t>COHERENCE FIBRES EN PASSAGE  VS PLAN DE SOUDURE</t>
+  </si>
+  <si>
+    <t>4.3.8</t>
+  </si>
+  <si>
+    <t>COHERENCE TUBES FOND DE BOITE VS PLAN DE SOUDURE</t>
+  </si>
+  <si>
+    <t>4.3.9</t>
+  </si>
+  <si>
+    <t>COHERENCE RANGEMENT DANS LES CASSETTES  VS PLAN DE SOUDURE</t>
   </si>
 </sst>
 </file>
@@ -1828,69 +1978,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1937,6 +2024,69 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2218,16 +2368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I264"/>
+  <dimension ref="A1:I295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="C270" sqref="C270"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="H275" sqref="H275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2303,7 +2453,7 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="60" t="s">
         <v>218</v>
       </c>
       <c r="D8" t="s">
@@ -2311,10 +2461,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="99"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -2429,10 +2579,10 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="100"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
@@ -2507,10 +2657,10 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="61"/>
+      <c r="C34" s="100"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
@@ -2524,7 +2674,7 @@
       <c r="A36" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="82" t="s">
+      <c r="B36" s="61" t="s">
         <v>64</v>
       </c>
       <c r="C36" t="s">
@@ -2535,12 +2685,12 @@
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
+      <c r="G36" s="101"/>
+      <c r="H36" s="101"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="61" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -2554,7 +2704,7 @@
       <c r="I37" s="59"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="61" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -2563,12 +2713,12 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="101"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="61" t="s">
         <v>70</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2577,12 +2727,12 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="64"/>
+      <c r="G39" s="102"/>
+      <c r="H39" s="103"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="82" t="s">
+      <c r="B40" s="61" t="s">
         <v>72</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2591,12 +2741,12 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="101"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="82" t="s">
+      <c r="B41" s="61" t="s">
         <v>74</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -2605,12 +2755,12 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="82" t="s">
+      <c r="B42" s="61" t="s">
         <v>76</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2619,12 +2769,12 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
+      <c r="G42" s="101"/>
+      <c r="H42" s="101"/>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="61" t="s">
         <v>78</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -2633,12 +2783,12 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="62"/>
+      <c r="G43" s="101"/>
+      <c r="H43" s="101"/>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="61" t="s">
         <v>80</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2647,12 +2797,12 @@
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
-      <c r="G44" s="67"/>
-      <c r="H44" s="68"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="96"/>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="82" t="s">
+      <c r="B45" s="61" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -2661,12 +2811,12 @@
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="68"/>
+      <c r="G45" s="95"/>
+      <c r="H45" s="96"/>
       <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="82" t="s">
+      <c r="B46" s="61" t="s">
         <v>84</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2675,12 +2825,12 @@
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="68"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="96"/>
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="82" t="s">
+      <c r="B47" s="61" t="s">
         <v>220</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2689,15 +2839,15 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="68"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="96"/>
       <c r="I47" s="12"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="82" t="s">
+      <c r="B48" s="61" t="s">
         <v>87</v>
       </c>
       <c r="C48" t="s">
@@ -2706,12 +2856,12 @@
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="70"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="86"/>
       <c r="I48" s="14"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="61" t="s">
         <v>89</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -2725,7 +2875,7 @@
       <c r="I49" s="57"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="61" t="s">
         <v>91</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -2734,12 +2884,12 @@
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="70"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="86"/>
       <c r="I50" s="14"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="61" t="s">
         <v>93</v>
       </c>
       <c r="C51" s="16" t="s">
@@ -2748,12 +2898,12 @@
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="72"/>
+      <c r="G51" s="89"/>
+      <c r="H51" s="90"/>
       <c r="I51" s="14"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="82" t="s">
+      <c r="B52" s="61" t="s">
         <v>95</v>
       </c>
       <c r="C52" s="16" t="s">
@@ -2762,12 +2912,12 @@
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="66"/>
+      <c r="G52" s="104"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="18"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="82" t="s">
+      <c r="B53" s="61" t="s">
         <v>97</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -2776,12 +2926,12 @@
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="71"/>
-      <c r="H53" s="72"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="90"/>
       <c r="I53" s="10"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="82" t="s">
+      <c r="B54" s="61" t="s">
         <v>99</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -2790,12 +2940,12 @@
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
-      <c r="G54" s="71"/>
-      <c r="H54" s="72"/>
+      <c r="G54" s="89"/>
+      <c r="H54" s="90"/>
       <c r="I54" s="10"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="61" t="s">
         <v>101</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -2804,12 +2954,12 @@
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="72"/>
+      <c r="G55" s="89"/>
+      <c r="H55" s="90"/>
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="61" t="s">
         <v>103</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2818,12 +2968,12 @@
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="70"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="86"/>
       <c r="I56" s="14"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="61" t="s">
         <v>105</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -2832,12 +2982,12 @@
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="71"/>
-      <c r="H57" s="72"/>
+      <c r="G57" s="89"/>
+      <c r="H57" s="90"/>
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="82" t="s">
+      <c r="B58" s="61" t="s">
         <v>107</v>
       </c>
       <c r="C58" s="7" t="s">
@@ -2846,12 +2996,12 @@
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="70"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="86"/>
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="82" t="s">
+      <c r="B59" s="61" t="s">
         <v>109</v>
       </c>
       <c r="C59" s="7" t="s">
@@ -2860,12 +3010,12 @@
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="70"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="86"/>
       <c r="I59" s="14"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="82" t="s">
+      <c r="B60" s="61" t="s">
         <v>111</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -2874,12 +3024,12 @@
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="69"/>
-      <c r="H60" s="70"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="86"/>
       <c r="I60" s="14"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="82" t="s">
+      <c r="B61" s="61" t="s">
         <v>113</v>
       </c>
       <c r="C61" s="15" t="s">
@@ -2888,12 +3038,12 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="74"/>
+      <c r="G61" s="97"/>
+      <c r="H61" s="98"/>
       <c r="I61" s="19"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="82" t="s">
+      <c r="B62" s="61" t="s">
         <v>115</v>
       </c>
       <c r="C62" s="20" t="s">
@@ -2907,7 +3057,7 @@
       <c r="I62" s="21"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="82" t="s">
+      <c r="B63" s="61" t="s">
         <v>118</v>
       </c>
       <c r="C63" s="20" t="s">
@@ -2921,16 +3071,16 @@
       <c r="I63" s="21"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="85" t="s">
+      <c r="B64" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C64" s="85"/>
-      <c r="D64" s="85"/>
-      <c r="E64" s="85"/>
-      <c r="F64" s="85"/>
-      <c r="G64" s="85"/>
-      <c r="H64" s="85"/>
-      <c r="I64" s="85"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
+      <c r="H64" s="64"/>
+      <c r="I64" s="64"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B65" s="13" t="s">
@@ -2942,21 +3092,21 @@
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
-      <c r="G65" s="69"/>
-      <c r="H65" s="70"/>
+      <c r="G65" s="85"/>
+      <c r="H65" s="86"/>
       <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="85" t="s">
+      <c r="B66" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="C66" s="85"/>
-      <c r="D66" s="85"/>
-      <c r="E66" s="85"/>
-      <c r="F66" s="85"/>
-      <c r="G66" s="85"/>
-      <c r="H66" s="85"/>
-      <c r="I66" s="85"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="64"/>
+      <c r="I66" s="64"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B67" s="13" t="s">
@@ -2968,24 +3118,24 @@
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="70"/>
+      <c r="G67" s="85"/>
+      <c r="H67" s="86"/>
       <c r="I67" s="14"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>123</v>
       </c>
-      <c r="B68" s="86" t="s">
+      <c r="B68" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="87"/>
-      <c r="D68" s="87"/>
-      <c r="E68" s="87"/>
-      <c r="F68" s="87"/>
-      <c r="G68" s="87"/>
-      <c r="H68" s="87"/>
-      <c r="I68" s="88"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="66"/>
+      <c r="I68" s="67"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B69" s="22" t="s">
@@ -2997,8 +3147,8 @@
       <c r="D69" s="24"/>
       <c r="E69" s="25"/>
       <c r="F69" s="26"/>
-      <c r="G69" s="76"/>
-      <c r="H69" s="77"/>
+      <c r="G69" s="93"/>
+      <c r="H69" s="94"/>
       <c r="I69" s="22"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3011,21 +3161,21 @@
       <c r="D70" s="28"/>
       <c r="E70" s="29"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
+      <c r="G70" s="91"/>
+      <c r="H70" s="91"/>
       <c r="I70" s="30"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="86" t="s">
+      <c r="B71" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="C71" s="87"/>
-      <c r="D71" s="87"/>
-      <c r="E71" s="87"/>
-      <c r="F71" s="87"/>
-      <c r="G71" s="87"/>
-      <c r="H71" s="87"/>
-      <c r="I71" s="88"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="67"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B72" s="22" t="s">
@@ -3037,8 +3187,8 @@
       <c r="D72" s="28"/>
       <c r="E72" s="31"/>
       <c r="F72" s="32"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
+      <c r="G72" s="91"/>
+      <c r="H72" s="91"/>
       <c r="I72" s="30"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3051,8 +3201,8 @@
       <c r="D73" s="28"/>
       <c r="E73" s="33"/>
       <c r="F73" s="34"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
+      <c r="G73" s="91"/>
+      <c r="H73" s="91"/>
       <c r="I73" s="30"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3065,8 +3215,8 @@
       <c r="D74" s="28"/>
       <c r="E74" s="28"/>
       <c r="F74" s="35"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
+      <c r="G74" s="91"/>
+      <c r="H74" s="91"/>
       <c r="I74" s="30"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3079,8 +3229,8 @@
       <c r="D75" s="28"/>
       <c r="E75" s="28"/>
       <c r="F75" s="37"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
+      <c r="G75" s="91"/>
+      <c r="H75" s="91"/>
       <c r="I75" s="30"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3093,21 +3243,21 @@
       <c r="D76" s="38"/>
       <c r="E76" s="16"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
+      <c r="G76" s="91"/>
+      <c r="H76" s="91"/>
       <c r="I76" s="30"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="86" t="s">
+      <c r="B77" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="87"/>
-      <c r="G77" s="87"/>
-      <c r="H77" s="87"/>
-      <c r="I77" s="87"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="66"/>
+      <c r="H77" s="66"/>
+      <c r="I77" s="66"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B78" s="22" t="s">
@@ -3119,8 +3269,8 @@
       <c r="D78" s="28"/>
       <c r="E78" s="29"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
+      <c r="G78" s="91"/>
+      <c r="H78" s="91"/>
       <c r="I78" s="30"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3133,8 +3283,8 @@
       <c r="D79" s="28"/>
       <c r="E79" s="41"/>
       <c r="F79" s="41"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
+      <c r="G79" s="91"/>
+      <c r="H79" s="91"/>
       <c r="I79" s="30"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3147,8 +3297,8 @@
       <c r="D80" s="43"/>
       <c r="E80" s="16"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
+      <c r="G80" s="91"/>
+      <c r="H80" s="91"/>
       <c r="I80" s="30"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
@@ -3160,8 +3310,8 @@
       </c>
       <c r="E81" s="16"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
+      <c r="G81" s="91"/>
+      <c r="H81" s="91"/>
       <c r="I81" s="30"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
@@ -3174,21 +3324,21 @@
       <c r="D82" s="45"/>
       <c r="E82" s="46"/>
       <c r="F82" s="46"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="78"/>
+      <c r="G82" s="92"/>
+      <c r="H82" s="92"/>
       <c r="I82" s="47"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="89" t="s">
+      <c r="B83" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="C83" s="85"/>
-      <c r="D83" s="85"/>
-      <c r="E83" s="85"/>
-      <c r="F83" s="85"/>
-      <c r="G83" s="85"/>
-      <c r="H83" s="85"/>
-      <c r="I83" s="90"/>
+      <c r="C83" s="64"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="69"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="22" t="s">
@@ -3200,8 +3350,8 @@
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
-      <c r="G84" s="71"/>
-      <c r="H84" s="72"/>
+      <c r="G84" s="89"/>
+      <c r="H84" s="90"/>
       <c r="I84" s="48"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
@@ -3214,8 +3364,8 @@
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="71"/>
-      <c r="H85" s="72"/>
+      <c r="G85" s="89"/>
+      <c r="H85" s="90"/>
       <c r="I85" s="48"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
@@ -3228,8 +3378,8 @@
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="71"/>
-      <c r="H86" s="72"/>
+      <c r="G86" s="89"/>
+      <c r="H86" s="90"/>
       <c r="I86" s="48"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
@@ -3242,8 +3392,8 @@
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
-      <c r="G87" s="71"/>
-      <c r="H87" s="72"/>
+      <c r="G87" s="89"/>
+      <c r="H87" s="90"/>
       <c r="I87" s="48"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
@@ -3256,8 +3406,8 @@
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
-      <c r="G88" s="71"/>
-      <c r="H88" s="72"/>
+      <c r="G88" s="89"/>
+      <c r="H88" s="90"/>
       <c r="I88" s="48"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
@@ -3270,8 +3420,8 @@
       <c r="D89" s="17"/>
       <c r="E89" s="17"/>
       <c r="F89" s="17"/>
-      <c r="G89" s="71"/>
-      <c r="H89" s="72"/>
+      <c r="G89" s="89"/>
+      <c r="H89" s="90"/>
       <c r="I89" s="48"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
@@ -3284,8 +3434,8 @@
       <c r="D90" s="17"/>
       <c r="E90" s="17"/>
       <c r="F90" s="17"/>
-      <c r="G90" s="71"/>
-      <c r="H90" s="72"/>
+      <c r="G90" s="89"/>
+      <c r="H90" s="90"/>
       <c r="I90" s="48"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
@@ -3298,8 +3448,8 @@
       <c r="D91" s="17"/>
       <c r="E91" s="17"/>
       <c r="F91" s="17"/>
-      <c r="G91" s="71"/>
-      <c r="H91" s="72"/>
+      <c r="G91" s="89"/>
+      <c r="H91" s="90"/>
       <c r="I91" s="48"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
@@ -3312,8 +3462,8 @@
       <c r="D92" s="17"/>
       <c r="E92" s="17"/>
       <c r="F92" s="17"/>
-      <c r="G92" s="71"/>
-      <c r="H92" s="72"/>
+      <c r="G92" s="89"/>
+      <c r="H92" s="90"/>
       <c r="I92" s="48"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
@@ -3326,8 +3476,8 @@
       <c r="D93" s="17"/>
       <c r="E93" s="17"/>
       <c r="F93" s="17"/>
-      <c r="G93" s="71"/>
-      <c r="H93" s="72"/>
+      <c r="G93" s="89"/>
+      <c r="H93" s="90"/>
       <c r="I93" s="48"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
@@ -3340,21 +3490,21 @@
       <c r="D94" s="17"/>
       <c r="E94" s="17"/>
       <c r="F94" s="17"/>
-      <c r="G94" s="71"/>
-      <c r="H94" s="72"/>
+      <c r="G94" s="89"/>
+      <c r="H94" s="90"/>
       <c r="I94" s="48"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="86" t="s">
+      <c r="B95" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="C95" s="87"/>
-      <c r="D95" s="87"/>
-      <c r="E95" s="87"/>
-      <c r="F95" s="87"/>
-      <c r="G95" s="87"/>
-      <c r="H95" s="87"/>
-      <c r="I95" s="87"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="66"/>
+      <c r="F95" s="66"/>
+      <c r="G95" s="66"/>
+      <c r="H95" s="66"/>
+      <c r="I95" s="66"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="22" t="s">
@@ -3366,8 +3516,8 @@
       <c r="D96" s="16"/>
       <c r="E96" s="16"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="75"/>
-      <c r="H96" s="75"/>
+      <c r="G96" s="91"/>
+      <c r="H96" s="91"/>
       <c r="I96" s="30"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3380,24 +3530,24 @@
       <c r="D97" s="16"/>
       <c r="E97" s="16"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="75"/>
-      <c r="H97" s="75"/>
+      <c r="G97" s="91"/>
+      <c r="H97" s="91"/>
       <c r="I97" s="30"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="85" t="s">
+      <c r="B98" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="C98" s="85"/>
-      <c r="D98" s="85"/>
-      <c r="E98" s="85"/>
-      <c r="F98" s="85"/>
-      <c r="G98" s="85"/>
-      <c r="H98" s="85"/>
-      <c r="I98" s="85"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="64"/>
+      <c r="G98" s="64"/>
+      <c r="H98" s="64"/>
+      <c r="I98" s="64"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B99" s="13" t="s">
@@ -3409,21 +3559,21 @@
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="70"/>
+      <c r="G99" s="85"/>
+      <c r="H99" s="86"/>
       <c r="I99" s="14"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="85" t="s">
+      <c r="B100" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="C100" s="85"/>
-      <c r="D100" s="85"/>
-      <c r="E100" s="85"/>
-      <c r="F100" s="85"/>
-      <c r="G100" s="85"/>
-      <c r="H100" s="85"/>
-      <c r="I100" s="85"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="64"/>
+      <c r="G100" s="64"/>
+      <c r="H100" s="64"/>
+      <c r="I100" s="64"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B101" s="13" t="s">
@@ -3435,8 +3585,8 @@
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
-      <c r="G101" s="71"/>
-      <c r="H101" s="72"/>
+      <c r="G101" s="89"/>
+      <c r="H101" s="90"/>
       <c r="I101" s="10"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -3449,8 +3599,8 @@
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
-      <c r="G102" s="69"/>
-      <c r="H102" s="70"/>
+      <c r="G102" s="85"/>
+      <c r="H102" s="86"/>
       <c r="I102" s="14"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3463,8 +3613,8 @@
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
-      <c r="G103" s="69"/>
-      <c r="H103" s="70"/>
+      <c r="G103" s="85"/>
+      <c r="H103" s="86"/>
       <c r="I103" s="14"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -3491,8 +3641,8 @@
       <c r="D105" s="53"/>
       <c r="E105" s="53"/>
       <c r="F105" s="53"/>
-      <c r="G105" s="79"/>
-      <c r="H105" s="80"/>
+      <c r="G105" s="87"/>
+      <c r="H105" s="88"/>
       <c r="I105" s="53"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -3524,16 +3674,16 @@
       <c r="I107" s="14"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="85" t="s">
+      <c r="B108" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="C108" s="85"/>
-      <c r="D108" s="85"/>
-      <c r="E108" s="85"/>
-      <c r="F108" s="85"/>
-      <c r="G108" s="85"/>
-      <c r="H108" s="85"/>
-      <c r="I108" s="85"/>
+      <c r="C108" s="64"/>
+      <c r="D108" s="64"/>
+      <c r="E108" s="64"/>
+      <c r="F108" s="64"/>
+      <c r="G108" s="64"/>
+      <c r="H108" s="64"/>
+      <c r="I108" s="64"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B109" s="13" t="s">
@@ -3545,8 +3695,8 @@
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
-      <c r="G109" s="69"/>
-      <c r="H109" s="70"/>
+      <c r="G109" s="85"/>
+      <c r="H109" s="86"/>
       <c r="I109" s="14"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -3559,21 +3709,21 @@
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
-      <c r="G110" s="69"/>
-      <c r="H110" s="70"/>
+      <c r="G110" s="85"/>
+      <c r="H110" s="86"/>
       <c r="I110" s="14"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="85" t="s">
+      <c r="B111" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="C111" s="85"/>
-      <c r="D111" s="85"/>
-      <c r="E111" s="85"/>
-      <c r="F111" s="85"/>
-      <c r="G111" s="85"/>
-      <c r="H111" s="85"/>
-      <c r="I111" s="85"/>
+      <c r="C111" s="64"/>
+      <c r="D111" s="64"/>
+      <c r="E111" s="64"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="64"/>
+      <c r="I111" s="64"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B112" s="13" t="s">
@@ -3585,8 +3735,8 @@
       <c r="D112" s="54"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
-      <c r="G112" s="71"/>
-      <c r="H112" s="72"/>
+      <c r="G112" s="89"/>
+      <c r="H112" s="90"/>
       <c r="I112" s="10"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -3599,8 +3749,8 @@
       <c r="D113" s="54"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
-      <c r="G113" s="71"/>
-      <c r="H113" s="72"/>
+      <c r="G113" s="89"/>
+      <c r="H113" s="90"/>
       <c r="I113" s="10"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -3613,8 +3763,8 @@
       <c r="D114" s="55"/>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
-      <c r="G114" s="71"/>
-      <c r="H114" s="72"/>
+      <c r="G114" s="89"/>
+      <c r="H114" s="90"/>
       <c r="I114" s="10"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -3627,21 +3777,21 @@
       <c r="D115" s="54"/>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
-      <c r="G115" s="71"/>
-      <c r="H115" s="72"/>
+      <c r="G115" s="89"/>
+      <c r="H115" s="90"/>
       <c r="I115" s="10"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="85" t="s">
+      <c r="B116" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="C116" s="85"/>
-      <c r="D116" s="85"/>
-      <c r="E116" s="85"/>
-      <c r="F116" s="85"/>
-      <c r="G116" s="85"/>
-      <c r="H116" s="85"/>
-      <c r="I116" s="85"/>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="64"/>
+      <c r="F116" s="64"/>
+      <c r="G116" s="64"/>
+      <c r="H116" s="64"/>
+      <c r="I116" s="64"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B117" s="13" t="s">
@@ -3653,8 +3803,8 @@
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
-      <c r="G117" s="69"/>
-      <c r="H117" s="70"/>
+      <c r="G117" s="85"/>
+      <c r="H117" s="86"/>
       <c r="I117" s="14"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -3683,10 +3833,10 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B120" s="83" t="s">
+      <c r="B120" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="C120" s="84"/>
+      <c r="C120" s="63"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B121" s="13" t="s">
@@ -3721,10 +3871,10 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="83" t="s">
+      <c r="B125" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="C125" s="84"/>
+      <c r="C125" s="63"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B126" s="13" t="s">
@@ -3735,10 +3885,10 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B127" s="83" t="s">
+      <c r="B127" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="C127" s="84"/>
+      <c r="C127" s="63"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B128" s="13" t="s">
@@ -3845,10 +3995,10 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="83" t="s">
+      <c r="B141" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C141" s="84"/>
+      <c r="C141" s="63"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B142" s="13" t="s">
@@ -3862,7 +4012,7 @@
       <c r="A143" t="s">
         <v>262</v>
       </c>
-      <c r="B143" s="93" t="s">
+      <c r="B143" s="72" t="s">
         <v>263</v>
       </c>
       <c r="C143" t="s">
@@ -3873,10 +4023,10 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="91" t="s">
+      <c r="B144" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="C144" s="92"/>
+      <c r="C144" s="71"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" s="13" t="s">
@@ -3911,10 +4061,10 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B149" s="91" t="s">
+      <c r="B149" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="C149" s="92"/>
+      <c r="C149" s="71"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" s="13" t="s">
@@ -3973,10 +4123,10 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B157" s="91" t="s">
+      <c r="B157" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="C157" s="92"/>
+      <c r="C157" s="71"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B158" s="13" t="s">
@@ -3990,16 +4140,16 @@
       <c r="A159" t="s">
         <v>284</v>
       </c>
-      <c r="B159" s="89" t="s">
+      <c r="B159" s="68" t="s">
         <v>285</v>
       </c>
-      <c r="C159" s="85"/>
+      <c r="C159" s="64"/>
     </row>
     <row r="160" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B160" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="C160" s="94" t="s">
+      <c r="C160" s="73" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4007,7 +4157,7 @@
       <c r="B161" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="C161" s="95" t="s">
+      <c r="C161" s="74" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4015,7 +4165,7 @@
       <c r="B162" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C162" s="94" t="s">
+      <c r="C162" s="73" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4023,7 +4173,7 @@
       <c r="B163" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C163" s="95" t="s">
+      <c r="C163" s="74" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4031,7 +4181,7 @@
       <c r="B164" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="C164" s="95" t="s">
+      <c r="C164" s="74" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4039,7 +4189,7 @@
       <c r="B165" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C165" s="95" t="s">
+      <c r="C165" s="74" t="s">
         <v>297</v>
       </c>
     </row>
@@ -4047,7 +4197,7 @@
       <c r="B166" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="C166" s="95" t="s">
+      <c r="C166" s="74" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4055,15 +4205,15 @@
       <c r="B167" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="C167" s="96" t="s">
+      <c r="C167" s="75" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="86" t="s">
+      <c r="B168" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="C168" s="87"/>
+      <c r="C168" s="66"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B169" s="13" t="s">
@@ -4077,7 +4227,7 @@
       <c r="B170" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="C170" s="97" t="s">
+      <c r="C170" s="76" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4093,21 +4243,21 @@
       <c r="B172" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="C172" s="97" t="s">
+      <c r="C172" s="76" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="86" t="s">
+      <c r="B173" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="C173" s="87"/>
+      <c r="C173" s="66"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B174" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="C174" s="98" t="s">
+      <c r="C174" s="77" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4137,16 +4287,16 @@
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" s="89" t="s">
+      <c r="B177" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="C177" s="85"/>
+      <c r="C177" s="64"/>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="C178" s="99" t="s">
+      <c r="C178" s="78" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4154,7 +4304,7 @@
       <c r="B179" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C179" s="99" t="s">
+      <c r="C179" s="78" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4162,7 +4312,7 @@
       <c r="B180" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="C180" s="99" t="s">
+      <c r="C180" s="78" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4170,7 +4320,7 @@
       <c r="B181" s="58" t="s">
         <v>316</v>
       </c>
-      <c r="C181" s="99" t="s">
+      <c r="C181" s="78" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4178,7 +4328,7 @@
       <c r="B182" s="58" t="s">
         <v>317</v>
       </c>
-      <c r="C182" s="99" t="s">
+      <c r="C182" s="78" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4186,7 +4336,7 @@
       <c r="B183" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="C183" s="99" t="s">
+      <c r="C183" s="78" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4194,7 +4344,7 @@
       <c r="B184" s="58" t="s">
         <v>319</v>
       </c>
-      <c r="C184" s="99" t="s">
+      <c r="C184" s="78" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4202,7 +4352,7 @@
       <c r="B185" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="C185" s="99" t="s">
+      <c r="C185" s="78" t="s">
         <v>251</v>
       </c>
     </row>
@@ -4210,21 +4360,21 @@
       <c r="B186" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="C186" s="99" t="s">
+      <c r="C186" s="78" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B187" s="86" t="s">
+      <c r="B187" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="C187" s="87"/>
+      <c r="C187" s="66"/>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="58" t="s">
         <v>325</v>
       </c>
-      <c r="C188" s="99" t="s">
+      <c r="C188" s="78" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4232,7 +4382,7 @@
       <c r="B189" s="58" t="s">
         <v>326</v>
       </c>
-      <c r="C189" s="99" t="s">
+      <c r="C189" s="78" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4240,7 +4390,7 @@
       <c r="B190" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="C190" s="99" t="s">
+      <c r="C190" s="78" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4248,7 +4398,7 @@
       <c r="B191" s="58" t="s">
         <v>329</v>
       </c>
-      <c r="C191" s="99" t="s">
+      <c r="C191" s="78" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4256,35 +4406,35 @@
       <c r="B192" s="58" t="s">
         <v>331</v>
       </c>
-      <c r="C192" s="99" t="s">
+      <c r="C192" s="78" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="86" t="s">
+      <c r="B193" s="65" t="s">
         <v>227</v>
       </c>
-      <c r="C193" s="87"/>
+      <c r="C193" s="66"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B194" s="58" t="s">
         <v>333</v>
       </c>
-      <c r="C194" s="99" t="s">
+      <c r="C194" s="78" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="86" t="s">
+      <c r="B195" s="65" t="s">
         <v>330</v>
       </c>
-      <c r="C195" s="87"/>
+      <c r="C195" s="66"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B196" s="58" t="s">
         <v>335</v>
       </c>
-      <c r="C196" s="99" t="s">
+      <c r="C196" s="78" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4300,7 +4450,7 @@
       <c r="B198" s="58" t="s">
         <v>339</v>
       </c>
-      <c r="C198" s="99" t="s">
+      <c r="C198" s="78" t="s">
         <v>336</v>
       </c>
     </row>
@@ -4308,7 +4458,7 @@
       <c r="B199" s="58" t="s">
         <v>341</v>
       </c>
-      <c r="C199" s="99" t="s">
+      <c r="C199" s="78" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4316,7 +4466,7 @@
       <c r="B200" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="C200" s="99" t="s">
+      <c r="C200" s="78" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4324,7 +4474,7 @@
       <c r="B201" s="58" t="s">
         <v>345</v>
       </c>
-      <c r="C201" s="99" t="s">
+      <c r="C201" s="78" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4332,7 +4482,7 @@
       <c r="B202" s="58" t="s">
         <v>347</v>
       </c>
-      <c r="C202" s="99" t="s">
+      <c r="C202" s="78" t="s">
         <v>344</v>
       </c>
     </row>
@@ -4340,21 +4490,21 @@
       <c r="B203" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="C203" s="99" t="s">
+      <c r="C203" s="78" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B204" s="86" t="s">
+      <c r="B204" s="65" t="s">
         <v>173</v>
       </c>
-      <c r="C204" s="87"/>
+      <c r="C204" s="66"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B205" s="58" t="s">
         <v>351</v>
       </c>
-      <c r="C205" s="98" t="s">
+      <c r="C205" s="77" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4384,16 +4534,16 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="100" t="s">
+      <c r="B208" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="C208" s="101"/>
+      <c r="C208" s="80"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="C209" s="99" t="s">
+      <c r="C209" s="78" t="s">
         <v>354</v>
       </c>
     </row>
@@ -4401,7 +4551,7 @@
       <c r="B210" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="C210" s="99" t="s">
+      <c r="C210" s="78" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4409,7 +4559,7 @@
       <c r="B211" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="C211" s="99" t="s">
+      <c r="C211" s="78" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4417,7 +4567,7 @@
       <c r="B212" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C212" s="99" t="s">
+      <c r="C212" s="78" t="s">
         <v>359</v>
       </c>
     </row>
@@ -4425,21 +4575,21 @@
       <c r="B213" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="C213" s="99" t="s">
+      <c r="C213" s="78" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="102" t="s">
+      <c r="B214" s="81" t="s">
         <v>361</v>
       </c>
-      <c r="C214" s="103"/>
+      <c r="C214" s="82"/>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="C215" s="99" t="s">
+      <c r="C215" s="78" t="s">
         <v>363</v>
       </c>
     </row>
@@ -4447,7 +4597,7 @@
       <c r="B216" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="C216" s="99" t="s">
+      <c r="C216" s="78" t="s">
         <v>365</v>
       </c>
     </row>
@@ -4455,21 +4605,21 @@
       <c r="B217" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="C217" s="99" t="s">
+      <c r="C217" s="78" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B218" s="89" t="s">
+      <c r="B218" s="68" t="s">
         <v>330</v>
       </c>
-      <c r="C218" s="85"/>
+      <c r="C218" s="64"/>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="C219" s="99" t="s">
+      <c r="C219" s="78" t="s">
         <v>354</v>
       </c>
     </row>
@@ -4485,7 +4635,7 @@
       <c r="B221" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="C221" s="99" t="s">
+      <c r="C221" s="78" t="s">
         <v>371</v>
       </c>
     </row>
@@ -4493,7 +4643,7 @@
       <c r="B222" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="C222" s="99" t="s">
+      <c r="C222" s="78" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4501,7 +4651,7 @@
       <c r="B223" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="C223" s="99" t="s">
+      <c r="C223" s="78" t="s">
         <v>340</v>
       </c>
     </row>
@@ -4509,7 +4659,7 @@
       <c r="B224" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="C224" s="99" t="s">
+      <c r="C224" s="78" t="s">
         <v>375</v>
       </c>
     </row>
@@ -4517,7 +4667,7 @@
       <c r="B225" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="C225" s="99" t="s">
+      <c r="C225" s="78" t="s">
         <v>344</v>
       </c>
     </row>
@@ -4525,21 +4675,21 @@
       <c r="B226" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="C226" s="99" t="s">
+      <c r="C226" s="78" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="89" t="s">
+      <c r="B227" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="C227" s="85"/>
+      <c r="C227" s="64"/>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="C228" s="99" t="s">
+      <c r="C228" s="78" t="s">
         <v>380</v>
       </c>
     </row>
@@ -4547,7 +4697,7 @@
       <c r="B229" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="C229" s="99" t="s">
+      <c r="C229" s="78" t="s">
         <v>382</v>
       </c>
     </row>
@@ -4555,7 +4705,7 @@
       <c r="B230" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="C230" s="104" t="s">
+      <c r="C230" s="83" t="s">
         <v>384</v>
       </c>
     </row>
@@ -4563,7 +4713,7 @@
       <c r="B231" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="C231" s="105" t="s">
+      <c r="C231" s="84" t="s">
         <v>386</v>
       </c>
     </row>
@@ -4600,16 +4750,16 @@
       </c>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B236" s="89" t="s">
+      <c r="B236" s="68" t="s">
         <v>395</v>
       </c>
-      <c r="C236" s="85"/>
+      <c r="C236" s="64"/>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="C237" s="99" t="s">
+      <c r="C237" s="78" t="s">
         <v>397</v>
       </c>
     </row>
@@ -4617,7 +4767,7 @@
       <c r="B238" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="C238" s="99" t="s">
+      <c r="C238" s="78" t="s">
         <v>399</v>
       </c>
     </row>
@@ -4625,7 +4775,7 @@
       <c r="B239" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="C239" s="99" t="s">
+      <c r="C239" s="78" t="s">
         <v>401</v>
       </c>
     </row>
@@ -4633,7 +4783,7 @@
       <c r="B240" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="C240" s="99" t="s">
+      <c r="C240" s="78" t="s">
         <v>403</v>
       </c>
     </row>
@@ -4641,7 +4791,7 @@
       <c r="B241" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="C241" s="99" t="s">
+      <c r="C241" s="78" t="s">
         <v>405</v>
       </c>
     </row>
@@ -4649,7 +4799,7 @@
       <c r="B242" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="C242" s="99" t="s">
+      <c r="C242" s="78" t="s">
         <v>407</v>
       </c>
     </row>
@@ -4657,7 +4807,7 @@
       <c r="B243" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="C243" s="99" t="s">
+      <c r="C243" s="78" t="s">
         <v>409</v>
       </c>
     </row>
@@ -4665,7 +4815,7 @@
       <c r="B244" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="C244" s="99" t="s">
+      <c r="C244" s="78" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4673,7 +4823,7 @@
       <c r="B245" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="C245" s="99" t="s">
+      <c r="C245" s="78" t="s">
         <v>413</v>
       </c>
     </row>
@@ -4686,16 +4836,16 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B247" s="89" t="s">
+      <c r="B247" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="C247" s="85"/>
+      <c r="C247" s="64"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B248" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="C248" s="28" t="s">
+      <c r="C248" s="49" t="s">
         <v>212</v>
       </c>
       <c r="D248" t="s">
@@ -4706,10 +4856,10 @@
       <c r="A249" t="s">
         <v>421</v>
       </c>
-      <c r="B249" s="93" t="s">
+      <c r="B249" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C249" s="49" t="s">
         <v>215</v>
       </c>
       <c r="D249" t="s">
@@ -4717,10 +4867,10 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="93" t="s">
+      <c r="B250" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C250" s="49" t="s">
         <v>423</v>
       </c>
       <c r="D250" t="s">
@@ -4728,10 +4878,10 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B251" s="93" t="s">
+      <c r="B251" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D251" t="s">
@@ -4739,10 +4889,10 @@
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="93" t="s">
+      <c r="B252" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="C252" t="s">
+      <c r="C252" s="49" t="s">
         <v>425</v>
       </c>
       <c r="D252" t="s">
@@ -4750,10 +4900,10 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B253" s="93" t="s">
+      <c r="B253" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C253" s="49" t="s">
         <v>430</v>
       </c>
     </row>
@@ -4761,10 +4911,10 @@
       <c r="A254" t="s">
         <v>431</v>
       </c>
-      <c r="B254" s="93" t="s">
+      <c r="B254" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C254" s="49" t="s">
         <v>215</v>
       </c>
       <c r="D254" t="s">
@@ -4772,10 +4922,10 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="93" t="s">
+      <c r="B255" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="49" t="s">
         <v>423</v>
       </c>
       <c r="D255" t="s">
@@ -4783,10 +4933,10 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B256" s="93" t="s">
+      <c r="B256" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C256" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D256" t="s">
@@ -4794,10 +4944,10 @@
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B257" s="93" t="s">
+      <c r="B257" s="13" t="s">
         <v>435</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C257" s="49" t="s">
         <v>425</v>
       </c>
       <c r="D257" t="s">
@@ -4805,10 +4955,10 @@
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="93" t="s">
+      <c r="B258" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C258" s="49" t="s">
         <v>437</v>
       </c>
     </row>
@@ -4816,10 +4966,10 @@
       <c r="A259" t="s">
         <v>438</v>
       </c>
-      <c r="B259" s="93" t="s">
+      <c r="B259" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C259" s="49" t="s">
         <v>215</v>
       </c>
       <c r="D259" t="s">
@@ -4827,10 +4977,10 @@
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B260" s="93" t="s">
+      <c r="B260" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C260" s="49" t="s">
         <v>423</v>
       </c>
       <c r="D260" t="s">
@@ -4838,10 +4988,10 @@
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B261" s="93" t="s">
+      <c r="B261" s="13" t="s">
         <v>441</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D261" t="s">
@@ -4849,10 +4999,10 @@
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B262" s="93" t="s">
+      <c r="B262" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="C262" t="s">
+      <c r="C262" s="49" t="s">
         <v>425</v>
       </c>
       <c r="D262" t="s">
@@ -4860,10 +5010,10 @@
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B263" s="93" t="s">
+      <c r="B263" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C263" s="49" t="s">
         <v>444</v>
       </c>
     </row>
@@ -4871,63 +5021,248 @@
       <c r="A264" t="s">
         <v>445</v>
       </c>
-      <c r="B264" s="93" t="s">
+      <c r="B264" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C264" s="49" t="s">
         <v>447</v>
       </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>448</v>
+      </c>
+      <c r="B265" s="68" t="s">
+        <v>449</v>
+      </c>
+      <c r="C265" s="68"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B266" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="C266" s="49" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C267" s="49" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B268" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C268" s="49" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B269" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="C269" s="68"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B270" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="C270" s="49" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B271" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="C271" s="49" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B272" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="C272" s="49" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B273" s="68" t="s">
+        <v>460</v>
+      </c>
+      <c r="C273" s="68"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B274" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="C274" s="49" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B275" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C275" s="49" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B276" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="C276" s="49" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B277" s="68" t="s">
+        <v>464</v>
+      </c>
+      <c r="C277" s="68"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B278" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="C278" s="49" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>470</v>
+      </c>
+      <c r="B279" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C279" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="D279" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B280" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C280" s="49" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B281" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="C281" s="49" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B282" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="C282" s="49" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>479</v>
+      </c>
+      <c r="B283" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="C283" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="D283" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B284" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C284" s="49" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B285" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="C285" s="49" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B286" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="C286" s="49" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B287" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="C287" s="49" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B288" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C288" s="49" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B289" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="C289" s="49" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B290" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="C290" s="49" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B291" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="C291" s="49" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C294" s="13"/>
+      <c r="D294" s="49"/>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C295" s="13"/>
+      <c r="D295" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="G105:H105"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="G99:H99"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
     <mergeCell ref="G59:H59"/>
     <mergeCell ref="G60:H60"/>
     <mergeCell ref="G61:H61"/>
@@ -4944,8 +5279,54 @@
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>